<commit_message>
fixes to summary formulas
</commit_message>
<xml_diff>
--- a/master_orders.xlsx
+++ b/master_orders.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8609C9E5-38C1-4BA8-AA06-4A34EDD111EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738EBBF5-B92B-4D6B-AE29-703BEA2E7A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4305" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="orders" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>No. of Items</t>
   </si>
@@ -55,10 +55,16 @@
     <t>S&amp;H Cost</t>
   </si>
   <si>
+    <t>Total Expenses</t>
+  </si>
+  <si>
+    <t>My Cost</t>
+  </si>
+  <si>
     <t>Total Profit</t>
   </si>
   <si>
-    <t>My Cost</t>
+    <t/>
   </si>
   <si>
     <t>ROI</t>
@@ -110,6 +116,12 @@
   </si>
   <si>
     <t>Date Sold</t>
+  </si>
+  <si>
+    <t>International Fees</t>
+  </si>
+  <si>
+    <t>Other Fee</t>
   </si>
 </sst>
 </file>
@@ -179,7 +191,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -190,12 +202,16 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -505,7 +521,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,7 +531,7 @@
     <col min="4" max="4" width="36.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" style="8" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
     <col min="9" max="9" width="14.85546875" customWidth="1"/>
     <col min="10" max="10" width="12.28515625" customWidth="1"/>
@@ -532,7 +548,7 @@
       <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="9">
+      <c r="F1" s="8">
         <f>COUNTA(A8:A1048576)</f>
         <v>0</v>
       </c>
@@ -540,7 +556,7 @@
         <v>1</v>
       </c>
       <c r="H1" s="2">
-        <f>SUM(J8:J451)</f>
+        <f>SUM(J8:J1048576)</f>
         <v>0</v>
       </c>
       <c r="I1" s="3" t="s">
@@ -556,21 +572,21 @@
         <v>3</v>
       </c>
       <c r="F2" s="2">
-        <f>SUM(F8:F451)</f>
+        <f>SUM(F8:F1048576)</f>
         <v>0</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="2">
-        <f>SUM(K8:K451)</f>
+        <f>SUM(K8:K1048576)</f>
         <v>0</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="J2" s="5">
-        <f>F4+H1+H2+H3</f>
+        <f>F4+H1+H2+H3+H4+H5</f>
         <v>0</v>
       </c>
     </row>
@@ -579,100 +595,125 @@
         <v>6</v>
       </c>
       <c r="F3" s="2">
-        <f>SUM(H8:H451)</f>
+        <f>SUM(H8:H1048576)</f>
         <v>0</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="H3" s="2">
-        <f>SUM(I8:I451)</f>
+        <f>SUM(L8:L1048576)</f>
         <v>0</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="5">
-        <f>J1+J2</f>
-        <v>0</v>
-      </c>
+      <c r="J3" s="10">
+        <v>0</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="2">
-        <f>SUM(E8:E451)</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="8"/>
+        <f>SUM(E8:E1048576)</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="2">
+        <f>SUM(M8:M1048576)</f>
+        <v>0</v>
+      </c>
       <c r="I4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="4" t="str">
-        <f>IFERROR(J3/J1," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="J4" s="5">
+        <f>J1+J2+J3</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="4"/>
+      <c r="C5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="2">
+        <f>SUM(I8:I1048576)</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="4" t="str">
+        <f>IFERROR(J4/J1," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G6" s="8"/>
+      <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:17" s="7" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" s="9" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -682,6 +723,6 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" verticalDpi="0"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>